<commit_message>
padding application with three execution models
</commit_message>
<xml_diff>
--- a/PAD/PAD_data.xlsx
+++ b/PAD/PAD_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="158">
   <si>
     <t>ALUTs</t>
   </si>
@@ -215,14 +215,6 @@
     <t>1,466 / 2,713 ( 54 % )</t>
   </si>
   <si>
-    <t>ul1_8_cu3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>basic(not_use_pmem)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>48,459 / 427,200 ( 11 % )</t>
   </si>
   <si>
@@ -543,6 +535,10 @@
   </si>
   <si>
     <t>use private memory for reg[40000]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_no_pmem</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -690,9 +686,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -707,6 +700,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:K17"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -999,15 +995,15 @@
     <col min="1" max="1" width="19.625" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
     <col min="7" max="7" width="10.625" customWidth="1"/>
-    <col min="9" max="10" width="9" style="16"/>
+    <col min="9" max="10" width="9" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="10.5">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B1" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1015,10 +1011,10 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="31.5">
       <c r="A2" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>0</v>
@@ -1038,7 +1034,7 @@
       <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="7" t="s">
@@ -1049,8 +1045,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A3" s="14" t="s">
-        <v>136</v>
+      <c r="A3" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1061,7 +1057,7 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A4" s="14"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1076,7 +1072,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A5" s="14"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1091,7 +1087,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="31.5">
-      <c r="A6" s="14"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1125,7 +1121,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A7" s="14"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1136,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A8" s="14"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1159,7 +1155,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C9" s="1">
         <v>154963</v>
@@ -1195,7 +1191,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C10" s="1">
         <v>181856</v>
@@ -1228,7 +1224,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C11" s="1">
         <v>207093</v>
@@ -1264,7 +1260,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C12" s="1">
         <v>161401</v>
@@ -1300,7 +1296,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C13" s="1">
         <v>208087</v>
@@ -1336,7 +1332,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C14" s="1">
         <v>249927</v>
@@ -1372,7 +1368,7 @@
         <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C15" s="1">
         <v>316059</v>
@@ -1408,7 +1404,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C16" s="1">
         <v>166518</v>
@@ -1444,12 +1440,12 @@
         <v>55</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C17" s="2">
         <v>213243</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <v>370406</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1476,12 +1472,6 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="1" customFormat="1" ht="10.5">
-      <c r="A18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="D18" s="9"/>
       <c r="I18" s="11"/>
       <c r="K18" s="3"/>
@@ -1496,493 +1486,527 @@
       <c r="I20" s="11"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:14" s="1" customFormat="1" ht="10.5">
-      <c r="D21" s="9"/>
-      <c r="I21" s="11"/>
+    <row r="21" spans="1:14" s="2" customFormat="1" ht="10.5">
+      <c r="A21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21" s="2">
+        <v>10</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:14" s="2" customFormat="1" ht="10.5">
-      <c r="A22" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" s="2">
-        <v>10</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="3"/>
+    <row r="22" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A22" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A23" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="A23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="1">
+        <v>60846</v>
+      </c>
+      <c r="D23" s="9">
+        <v>79595</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="11">
+        <v>370</v>
+      </c>
+      <c r="J23" s="1">
+        <v>35.223999999999997</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" ref="K23:K32" si="1">MMULT(I23,J23)*1000</f>
+        <v>13032880</v>
+      </c>
+      <c r="N23" s="12"/>
     </row>
     <row r="24" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="C24" s="1">
-        <v>60846</v>
+        <v>59113</v>
       </c>
       <c r="D24" s="9">
-        <v>79595</v>
+        <v>78057</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I24" s="11">
-        <v>370</v>
+        <v>248.333333334</v>
       </c>
       <c r="J24" s="1">
-        <v>35.223999999999997</v>
+        <v>0.753</v>
       </c>
       <c r="K24" s="3">
-        <f>MMULT(I24,J24)*1000</f>
-        <v>13032880</v>
+        <f t="shared" si="1"/>
+        <v>186995.00000050198</v>
       </c>
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="1">
+        <v>60492</v>
+      </c>
+      <c r="D25" s="9">
+        <v>79951</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C25" s="1">
-        <v>59113</v>
-      </c>
-      <c r="D25" s="9">
-        <v>78057</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I25" s="11">
-        <v>248.333333334</v>
+        <v>214.583333334</v>
       </c>
       <c r="J25" s="1">
-        <v>0.753</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="K25" s="3">
-        <f>MMULT(I25,J25)*1000</f>
-        <v>186995.00000050198</v>
-      </c>
-      <c r="N25" s="12"/>
-    </row>
-    <row r="26" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A26" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="1">
-        <v>60492</v>
-      </c>
-      <c r="D26" s="9">
-        <v>79951</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G26" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>122312.50000037998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="2" customFormat="1" ht="31.5">
+      <c r="A26" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="B26" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="2">
+        <v>63994</v>
+      </c>
+      <c r="D26" s="16">
+        <v>85017</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I26" s="11">
-        <v>214.583333334</v>
-      </c>
-      <c r="J26" s="1">
-        <v>0.56999999999999995</v>
+      <c r="F26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="10">
+        <v>232.5</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.53400000000000003</v>
       </c>
       <c r="K26" s="3">
-        <f>MMULT(I26,J26)*1000</f>
-        <v>122312.50000037998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="2" customFormat="1" ht="31.5">
-      <c r="A27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C27" s="2">
-        <v>63994</v>
-      </c>
-      <c r="D27" s="17">
-        <v>85017</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>124155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="B27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="1">
+        <v>70611</v>
+      </c>
+      <c r="D27" s="9">
+        <v>93102</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I27" s="10">
-        <v>232.5</v>
-      </c>
-      <c r="J27" s="2">
-        <v>0.53400000000000003</v>
+      <c r="F27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="11">
+        <v>196.25</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.60499999999999998</v>
       </c>
       <c r="K27" s="3">
-        <f>MMULT(I27,J27)*1000</f>
-        <v>124155</v>
+        <f t="shared" si="1"/>
+        <v>118731.25</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C28" s="1">
-        <v>70611</v>
+        <v>81651</v>
       </c>
       <c r="D28" s="9">
-        <v>93102</v>
+        <v>106906</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I28" s="11">
-        <v>196.25</v>
+        <v>162.5</v>
       </c>
       <c r="J28" s="1">
-        <v>0.60499999999999998</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="K28" s="3">
-        <f>MMULT(I28,J28)*1000</f>
-        <v>118731.25</v>
+        <f t="shared" si="1"/>
+        <v>106762.5</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C29" s="1">
-        <v>81651</v>
+        <v>103399</v>
       </c>
       <c r="D29" s="9">
-        <v>106906</v>
+        <v>134667</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I29" s="11">
-        <v>162.5</v>
+        <v>161.666666666</v>
       </c>
       <c r="J29" s="1">
-        <v>0.65700000000000003</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="K29" s="3">
-        <f>MMULT(I29,J29)*1000</f>
-        <v>106762.5</v>
+        <f t="shared" si="1"/>
+        <v>102658.33333291</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C30" s="1">
-        <v>103399</v>
+        <v>139557</v>
       </c>
       <c r="D30" s="9">
-        <v>134667</v>
+        <v>198676</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I30" s="11">
-        <v>161.666666666</v>
+        <v>154</v>
       </c>
       <c r="J30" s="1">
-        <v>0.63500000000000001</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="K30" s="3">
-        <f>MMULT(I30,J30)*1000</f>
-        <v>102658.33333291</v>
+        <f t="shared" si="1"/>
+        <v>106568</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A31" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C31" s="1">
-        <v>139557</v>
+        <v>80323</v>
       </c>
       <c r="D31" s="9">
-        <v>198676</v>
+        <v>116225</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I31" s="11">
-        <v>154</v>
+        <v>206.25</v>
       </c>
       <c r="J31" s="1">
-        <v>0.69199999999999995</v>
+        <v>12.811999999999999</v>
       </c>
       <c r="K31" s="3">
-        <f>MMULT(I31,J31)*1000</f>
-        <v>106568</v>
+        <f t="shared" si="1"/>
+        <v>2642475</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A32" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="1">
+        <v>109253</v>
+      </c>
+      <c r="D32" s="9">
+        <v>163683</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="11">
+        <v>196.875</v>
+      </c>
+      <c r="J32" s="1">
+        <v>13.288</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="1"/>
+        <v>2616075.0000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="2" customFormat="1" ht="10.5">
+      <c r="A36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="2">
+        <v>14</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:17" s="1" customFormat="1" ht="31.5">
+      <c r="A37" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C32" s="1">
-        <v>80323</v>
-      </c>
-      <c r="D32" s="9">
-        <v>116225</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I32" s="11">
-        <v>206.25</v>
-      </c>
-      <c r="J32" s="1">
-        <v>12.811999999999999</v>
-      </c>
-      <c r="K32" s="3">
-        <f>MMULT(I32,J32)*1000</f>
-        <v>2642475</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" s="1" customFormat="1" ht="31.5">
-      <c r="A33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C33" s="1">
-        <v>109253</v>
-      </c>
-      <c r="D33" s="9">
-        <v>163683</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="B37" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="13" customFormat="1" ht="31.5">
+      <c r="A38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="1">
+        <v>57120</v>
+      </c>
+      <c r="D38" s="9">
+        <v>70745</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="F38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I33" s="11">
-        <v>196.875</v>
-      </c>
-      <c r="J33" s="1">
-        <v>13.288</v>
-      </c>
-      <c r="K33" s="3">
-        <f>MMULT(I33,J33)*1000</f>
-        <v>2616075.0000000005</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" s="2" customFormat="1" ht="10.5">
-      <c r="A37" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B37" s="2">
-        <v>14</v>
-      </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="3"/>
-    </row>
-    <row r="38" spans="1:17" s="1" customFormat="1" ht="31.5">
-      <c r="A38" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="H38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I38" s="11">
+        <v>359.375</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="K38" s="3">
+        <f t="shared" ref="K38:K51" si="2">MMULT(I38,J38)*1000</f>
+        <v>73312.5</v>
+      </c>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
     </row>
     <row r="39" spans="1:17" s="13" customFormat="1" ht="31.5">
       <c r="A39" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C39" s="1">
-        <v>57120</v>
+        <v>61192</v>
       </c>
       <c r="D39" s="9">
-        <v>70745</v>
+        <v>79983</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I39" s="11">
-        <v>359.375</v>
+        <v>365.625</v>
       </c>
       <c r="J39" s="1">
-        <v>0.20399999999999999</v>
+        <v>0.185</v>
       </c>
       <c r="K39" s="3">
-        <f>MMULT(I39,J39)*1000</f>
-        <v>73312.5</v>
+        <f t="shared" si="2"/>
+        <v>67640.625</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -1993,442 +2017,403 @@
     </row>
     <row r="40" spans="1:17" s="13" customFormat="1" ht="31.5">
       <c r="A40" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="C40" s="1">
-        <v>61192</v>
+        <v>60726</v>
       </c>
       <c r="D40" s="9">
-        <v>79983</v>
+        <v>80044</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I40" s="11">
-        <v>365.625</v>
+        <v>366.66666666700002</v>
       </c>
       <c r="J40" s="1">
-        <v>0.185</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="K40" s="3">
-        <f>MMULT(I40,J40)*1000</f>
-        <v>67640.625</v>
-      </c>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
+        <f t="shared" si="2"/>
+        <v>103766.666666761</v>
+      </c>
     </row>
     <row r="41" spans="1:17" s="13" customFormat="1" ht="31.5">
       <c r="A41" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C41" s="1">
-        <v>60726</v>
+        <v>60274</v>
       </c>
       <c r="D41" s="9">
-        <v>80044</v>
+        <v>77806</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I41" s="11">
-        <v>366.66666666700002</v>
+        <v>379.16666666700002</v>
       </c>
       <c r="J41" s="1">
-        <v>0.28299999999999997</v>
+        <v>0.217</v>
       </c>
       <c r="K41" s="3">
-        <f>MMULT(I41,J41)*1000</f>
-        <v>103766.666666761</v>
+        <f t="shared" si="2"/>
+        <v>82279.166666739009</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="13" customFormat="1" ht="31.5">
       <c r="A42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="1">
+        <v>60400</v>
+      </c>
+      <c r="D42" s="9">
+        <v>78052</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I42" s="11">
+        <v>266.66666666700002</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K42" s="3">
+        <f t="shared" si="2"/>
+        <v>149333.33333352002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="31.5">
+      <c r="A43" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C42" s="1">
-        <v>60274</v>
-      </c>
-      <c r="D42" s="9">
-        <v>77806</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="C43" s="1">
+        <v>60312</v>
+      </c>
+      <c r="D43" s="9">
+        <v>77950</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I42" s="11">
-        <v>379.16666666700002</v>
-      </c>
-      <c r="J42" s="1">
-        <v>0.217</v>
-      </c>
-      <c r="K42" s="3">
-        <f>MMULT(I42,J42)*1000</f>
-        <v>82279.166666739009</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" s="13" customFormat="1" ht="31.5">
-      <c r="A43" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C43" s="1">
-        <v>60400</v>
-      </c>
-      <c r="D43" s="9">
-        <v>78052</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="I43" s="11">
-        <v>266.66666666700002</v>
+        <v>370</v>
       </c>
       <c r="J43" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="K43" s="3">
-        <f>MMULT(I43,J43)*1000</f>
-        <v>149333.33333352002</v>
+        <f t="shared" si="2"/>
+        <v>71040</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="31.5">
       <c r="A44" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C44" s="1">
-        <v>60312</v>
+        <v>60520</v>
       </c>
       <c r="D44" s="9">
-        <v>77950</v>
+        <v>78139</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I44" s="11">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="J44" s="1">
-        <v>0.192</v>
+        <v>0.184</v>
       </c>
       <c r="K44" s="3">
-        <f>MMULT(I44,J44)*1000</f>
-        <v>71040</v>
+        <f t="shared" si="2"/>
+        <v>69000</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="31.5">
       <c r="A45" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C45" s="1">
-        <v>60520</v>
+        <v>60338</v>
       </c>
       <c r="D45" s="9">
-        <v>78139</v>
+        <v>77985</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I45" s="11">
-        <v>375</v>
+        <v>365.625</v>
       </c>
       <c r="J45" s="1">
-        <v>0.184</v>
+        <v>0.2</v>
       </c>
       <c r="K45" s="3">
-        <f>MMULT(I45,J45)*1000</f>
-        <v>69000</v>
+        <f t="shared" si="2"/>
+        <v>73125</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="31.5">
       <c r="A46" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C46" s="1">
-        <v>60338</v>
+        <v>60344</v>
       </c>
       <c r="D46" s="9">
-        <v>77985</v>
+        <v>77994</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I46" s="11">
+        <v>362.5</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.184</v>
+      </c>
+      <c r="K46" s="3">
+        <f t="shared" si="2"/>
+        <v>66700</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" s="18" customFormat="1" ht="31.5">
+      <c r="A47" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="2">
+        <v>60377</v>
+      </c>
+      <c r="D47" s="16">
+        <v>78027</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I47" s="10">
+        <v>385</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="K47" s="3">
+        <f t="shared" si="2"/>
+        <v>68530</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="31.5">
+      <c r="A48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="1">
+        <v>60287</v>
+      </c>
+      <c r="D48" s="9">
+        <v>77984</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I48" s="11">
         <v>365.625</v>
       </c>
-      <c r="J46" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="K46" s="3">
-        <f>MMULT(I46,J46)*1000</f>
-        <v>73125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="31.5">
-      <c r="A47" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C47" s="1">
-        <v>60344</v>
-      </c>
-      <c r="D47" s="9">
-        <v>77994</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I47" s="11">
-        <v>362.5</v>
-      </c>
-      <c r="J47" s="1">
+      <c r="J48" s="1">
         <v>0.184</v>
       </c>
-      <c r="K47" s="3">
-        <f>MMULT(I47,J47)*1000</f>
-        <v>66700</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" s="19" customFormat="1" ht="31.5">
-      <c r="A48" s="2" t="s">
+      <c r="K48" s="3">
+        <f t="shared" si="2"/>
+        <v>67275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="1" customFormat="1" ht="31.5">
+      <c r="A49" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C48" s="2">
-        <v>60377</v>
-      </c>
-      <c r="D48" s="17">
-        <v>78027</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I48" s="10">
-        <v>385</v>
-      </c>
-      <c r="J48" s="2">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="K48" s="3">
-        <f>MMULT(I48,J48)*1000</f>
-        <v>68530</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="31.5">
-      <c r="A49" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="C49" s="1">
-        <v>60287</v>
+        <v>61362</v>
       </c>
       <c r="D49" s="9">
-        <v>77984</v>
+        <v>80259</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="I49" s="11">
-        <v>365.625</v>
+        <v>378.125</v>
       </c>
       <c r="J49" s="1">
-        <v>0.184</v>
+        <v>0.185</v>
       </c>
       <c r="K49" s="3">
-        <f>MMULT(I49,J49)*1000</f>
-        <v>67275</v>
+        <f t="shared" si="2"/>
+        <v>69953.125</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="1" customFormat="1" ht="31.5">
       <c r="A50" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C50" s="1">
-        <v>61362</v>
+        <v>61272</v>
       </c>
       <c r="D50" s="9">
-        <v>80259</v>
+        <v>80216</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>131</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>132</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I50" s="11">
-        <v>378.125</v>
+        <v>371.875</v>
       </c>
       <c r="J50" s="1">
-        <v>0.185</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="K50" s="3">
-        <f>MMULT(I50,J50)*1000</f>
-        <v>69953.125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" ht="31.5">
-      <c r="A51" s="1" t="s">
-        <v>157</v>
+        <f t="shared" si="2"/>
+        <v>75118.75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="31.5">
+      <c r="A51" s="17" t="s">
+        <v>151</v>
       </c>
       <c r="C51" s="1">
-        <v>61272</v>
+        <v>62027</v>
       </c>
       <c r="D51" s="9">
-        <v>80216</v>
+        <v>79659</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="I51" s="11">
-        <v>371.875</v>
+        <v>365.625</v>
       </c>
       <c r="J51" s="1">
-        <v>0.20200000000000001</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="K51" s="3">
-        <f>MMULT(I51,J51)*1000</f>
-        <v>75118.75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="31.5">
-      <c r="A52" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="1">
-        <v>62027</v>
-      </c>
-      <c r="D52" s="9">
-        <v>79659</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I52" s="11">
-        <v>365.625</v>
-      </c>
-      <c r="J52" s="1">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="K52" s="3">
-        <f>MMULT(I52,J52)*1000</f>
+        <f t="shared" si="2"/>
         <v>72759.375</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimize SWI and SWI+C of CEDD application
</commit_message>
<xml_diff>
--- a/PAD/PAD_data.xlsx
+++ b/PAD/PAD_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="163">
   <si>
     <t>ALUTs</t>
   </si>
@@ -539,6 +539,23 @@
   </si>
   <si>
     <t>basic_no_pmem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37,619 / 427,200 ( 9 % )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 / 1,518 ( 0 % )</t>
+  </si>
+  <si>
+    <t>1,993,744 / 55,562,240 ( 4 % )</t>
+  </si>
+  <si>
+    <t>228 / 2,713 ( 8 % )</t>
+  </si>
+  <si>
+    <t>null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -549,7 +566,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,6 +600,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -643,7 +666,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -666,9 +689,6 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -703,6 +723,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -984,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -995,7 +1030,7 @@
     <col min="1" max="1" width="19.625" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
     <col min="7" max="7" width="10.625" customWidth="1"/>
-    <col min="9" max="10" width="9" style="15"/>
+    <col min="9" max="11" width="9" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="10.5">
@@ -1007,7 +1042,7 @@
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="3"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="31.5">
       <c r="A2" s="4" t="s">
@@ -1034,18 +1069,18 @@
       <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1054,47 +1089,47 @@
       <c r="J3" s="1">
         <v>1.476</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="I4" s="11"/>
+      <c r="D4" s="8"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="1">
         <v>1.006</v>
       </c>
-      <c r="K4" s="3" t="e">
+      <c r="K4" s="11" t="e">
         <f>MMULT(I4,J4)*1000</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="I5" s="11"/>
+      <c r="D5" s="8"/>
+      <c r="I5" s="10"/>
       <c r="J5" s="1">
         <v>0.96299999999999997</v>
       </c>
-      <c r="K5" s="3" t="e">
+      <c r="K5" s="11" t="e">
         <f>MMULT(I5,J5)*1000</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="31.5">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>116462</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>168638</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1109,43 +1144,43 @@
       <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>223.333333334</v>
       </c>
       <c r="J6" s="1">
         <v>0.85399999999999998</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="11">
         <f>MMULT(I6,J6)*1000</f>
         <v>190726.66666723602</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A7" s="19"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="I7" s="11"/>
+      <c r="D7" s="8"/>
+      <c r="I7" s="10"/>
       <c r="J7" s="1">
         <v>0.96799999999999997</v>
       </c>
-      <c r="K7" s="3" t="e">
+      <c r="K7" s="11" t="e">
         <f>MMULT(I7,J7)*1000</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="10.5">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="I8" s="11"/>
+      <c r="D8" s="8"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="1">
         <v>0.97099999999999997</v>
       </c>
-      <c r="K8" s="3" t="e">
+      <c r="K8" s="11" t="e">
         <f>MMULT(I8,J8)*1000</f>
         <v>#VALUE!</v>
       </c>
@@ -1160,7 +1195,7 @@
       <c r="C9" s="1">
         <v>154963</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>217401</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1175,13 +1210,13 @@
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>235</v>
       </c>
       <c r="J9" s="1">
         <v>0.77400000000000002</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="11">
         <f t="shared" ref="K9:K17" si="0">MMULT(I9,J9)*1000</f>
         <v>181890.00000000003</v>
       </c>
@@ -1196,7 +1231,7 @@
       <c r="C10" s="1">
         <v>181856</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>245389</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1211,10 +1246,10 @@
       <c r="H10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>220.833333334</v>
       </c>
-      <c r="K10" s="3" t="e">
+      <c r="K10" s="11" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -1229,7 +1264,7 @@
       <c r="C11" s="1">
         <v>207093</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>268609</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1244,13 +1279,13 @@
       <c r="H11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>237.5</v>
       </c>
       <c r="J11" s="1">
         <v>0.86399999999999999</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="11">
         <f t="shared" si="0"/>
         <v>205200</v>
       </c>
@@ -1265,7 +1300,7 @@
       <c r="C12" s="1">
         <v>161401</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>255926</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1280,13 +1315,13 @@
       <c r="H12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>235.416666666</v>
       </c>
       <c r="J12" s="1">
         <v>0.876</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="11">
         <f t="shared" si="0"/>
         <v>206224.99999941597</v>
       </c>
@@ -1301,7 +1336,7 @@
       <c r="C13" s="1">
         <v>208087</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>348170</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1316,13 +1351,13 @@
       <c r="H13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>239.583333334</v>
       </c>
       <c r="J13" s="1">
         <v>0.78400000000000003</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="11">
         <f t="shared" si="0"/>
         <v>187833.33333385602</v>
       </c>
@@ -1337,7 +1372,7 @@
       <c r="C14" s="1">
         <v>249927</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>436319</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1352,13 +1387,13 @@
       <c r="H14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="10">
         <v>216.666666666</v>
       </c>
       <c r="J14" s="1">
         <v>0.84799999999999998</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="11">
         <f t="shared" si="0"/>
         <v>183733.33333276797</v>
       </c>
@@ -1373,7 +1408,7 @@
       <c r="C15" s="1">
         <v>316059</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>528887</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1388,13 +1423,13 @@
       <c r="H15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <v>179.166666666</v>
       </c>
       <c r="J15" s="1">
         <v>0.77100000000000002</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="11">
         <f t="shared" si="0"/>
         <v>138137.499999486</v>
       </c>
@@ -1409,7 +1444,7 @@
       <c r="C16" s="1">
         <v>166518</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>271303</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1424,13 +1459,13 @@
       <c r="H16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>215.625</v>
       </c>
       <c r="J16" s="1">
         <v>0.82499999999999996</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="11">
         <f t="shared" si="0"/>
         <v>177890.625</v>
       </c>
@@ -1445,7 +1480,7 @@
       <c r="C17" s="2">
         <v>213243</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="15">
         <v>370406</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1460,7 +1495,7 @@
       <c r="H17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>220</v>
       </c>
       <c r="J17" s="2">
@@ -1472,19 +1507,19 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="1" customFormat="1" ht="10.5">
-      <c r="D18" s="9"/>
-      <c r="I18" s="11"/>
-      <c r="K18" s="3"/>
+      <c r="D18" s="8"/>
+      <c r="I18" s="10"/>
+      <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:14" s="1" customFormat="1" ht="10.5">
-      <c r="D19" s="9"/>
-      <c r="I19" s="11"/>
-      <c r="K19" s="3"/>
+      <c r="D19" s="8"/>
+      <c r="I19" s="10"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" ht="10.5">
-      <c r="D20" s="9"/>
-      <c r="I20" s="11"/>
-      <c r="K20" s="3"/>
+      <c r="D20" s="8"/>
+      <c r="I20" s="10"/>
+      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" ht="10.5">
       <c r="A21" s="2" t="s">
@@ -1495,7 +1530,7 @@
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="3"/>
+      <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A22" s="4" t="s">
@@ -1522,897 +1557,934 @@
       <c r="H22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="13" t="s">
         <v>6</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K22" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A23" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C23" s="1">
-        <v>60846</v>
-      </c>
-      <c r="D23" s="9">
-        <v>79595</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="11">
-        <v>370</v>
-      </c>
-      <c r="J23" s="1">
-        <v>35.223999999999997</v>
-      </c>
-      <c r="K23" s="3">
-        <f t="shared" ref="K23:K32" si="1">MMULT(I23,J23)*1000</f>
-        <v>13032880</v>
-      </c>
-      <c r="N23" s="12"/>
+    <row r="23" spans="1:14" s="20" customFormat="1" ht="31.5">
+      <c r="A23" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="20">
+        <v>44887</v>
+      </c>
+      <c r="D23" s="21">
+        <v>53978</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" s="22">
+        <v>412.5</v>
+      </c>
+      <c r="J23" s="20">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K23" s="23">
+        <f>MMULT(I23,J23)*1000</f>
+        <v>27225</v>
+      </c>
     </row>
     <row r="24" spans="1:14" s="1" customFormat="1" ht="31.5">
       <c r="A24" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="1">
+        <v>60846</v>
+      </c>
+      <c r="D24" s="8">
+        <v>79595</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="10">
+        <v>370</v>
+      </c>
+      <c r="J24" s="1">
+        <v>35.223999999999997</v>
+      </c>
+      <c r="K24" s="11">
+        <f t="shared" ref="K23:K33" si="1">MMULT(I24,J24)*1000</f>
+        <v>13032880</v>
+      </c>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C25" s="1">
         <v>59113</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D25" s="8">
         <v>78057</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I25" s="10">
         <v>248.333333334</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J25" s="1">
         <v>0.753</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K25" s="11">
         <f t="shared" si="1"/>
         <v>186995.00000050198</v>
       </c>
-      <c r="N24" s="12"/>
-    </row>
-    <row r="25" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A25" s="1" t="s">
+      <c r="L25" s="11">
+        <f>K25-K23</f>
+        <v>159770.00000050198</v>
+      </c>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>60492</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D26" s="8">
         <v>79951</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I26" s="10">
         <v>214.583333334</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J26" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K26" s="11">
         <f t="shared" si="1"/>
         <v>122312.50000037998</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="2" customFormat="1" ht="31.5">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:14" s="2" customFormat="1" ht="31.5">
+      <c r="A27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C27" s="2">
         <v>63994</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D27" s="15">
         <v>85017</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I27" s="9">
         <v>232.5</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J27" s="2">
         <v>0.53400000000000003</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K27" s="3">
         <f t="shared" si="1"/>
         <v>124155</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
         <v>70611</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D28" s="8">
         <v>93102</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I28" s="10">
         <v>196.25</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J28" s="1">
         <v>0.60499999999999998</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K28" s="11">
         <f t="shared" si="1"/>
         <v>118731.25</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <v>81651</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D29" s="8">
         <v>106906</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="11">
+      <c r="I29" s="10">
         <v>162.5</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J29" s="1">
         <v>0.65700000000000003</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K29" s="11">
         <f t="shared" si="1"/>
         <v>106762.5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <v>103399</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D30" s="8">
         <v>134667</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I30" s="10">
         <v>161.666666666</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J30" s="1">
         <v>0.63500000000000001</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K30" s="11">
         <f t="shared" si="1"/>
         <v>102658.33333291</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C31" s="1">
         <v>139557</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D31" s="8">
         <v>198676</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I30" s="11">
+      <c r="I31" s="10">
         <v>154</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J31" s="1">
         <v>0.69199999999999995</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K31" s="11">
         <f t="shared" si="1"/>
         <v>106568</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:14" s="1" customFormat="1" ht="31.5">
+      <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C32" s="1">
         <v>80323</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D32" s="8">
         <v>116225</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I32" s="10">
         <v>206.25</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J32" s="1">
         <v>12.811999999999999</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K32" s="11">
         <f t="shared" si="1"/>
         <v>2642475</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="1" customFormat="1" ht="31.5">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:17" s="1" customFormat="1" ht="31.5">
+      <c r="A33" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <v>109253</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D33" s="8">
         <v>163683</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I32" s="11">
+      <c r="I33" s="10">
         <v>196.875</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J33" s="1">
         <v>13.288</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K33" s="11">
         <f t="shared" si="1"/>
         <v>2616075.0000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="2" customFormat="1" ht="10.5">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:17" s="2" customFormat="1" ht="10.5">
+      <c r="A37" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B37" s="2">
         <v>14</v>
       </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="3"/>
-    </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" ht="31.5">
-      <c r="A37" s="4" t="s">
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="11"/>
+    </row>
+    <row r="38" spans="1:17" s="1" customFormat="1" ht="31.5">
+      <c r="A38" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I38" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="7" t="s">
+      <c r="J38" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K37" s="8" t="s">
+      <c r="K38" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="13" customFormat="1" ht="31.5">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:17" s="12" customFormat="1" ht="31.5">
+      <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C39" s="1">
         <v>57120</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D39" s="8">
         <v>70745</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I38" s="11">
+      <c r="I39" s="10">
         <v>359.375</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J39" s="1">
         <v>0.20399999999999999</v>
       </c>
-      <c r="K38" s="3">
-        <f t="shared" ref="K38:K51" si="2">MMULT(I38,J38)*1000</f>
+      <c r="K39" s="11">
+        <f t="shared" ref="K39:K52" si="2">MMULT(I39,J39)*1000</f>
         <v>73312.5</v>
-      </c>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-    </row>
-    <row r="39" spans="1:17" s="13" customFormat="1" ht="31.5">
-      <c r="A39" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C39" s="1">
-        <v>61192</v>
-      </c>
-      <c r="D39" s="9">
-        <v>79983</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I39" s="11">
-        <v>365.625</v>
-      </c>
-      <c r="J39" s="1">
-        <v>0.185</v>
-      </c>
-      <c r="K39" s="3">
-        <f t="shared" si="2"/>
-        <v>67640.625</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="12"/>
+      <c r="N39" s="11"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" s="13" customFormat="1" ht="31.5">
+    <row r="40" spans="1:17" s="12" customFormat="1" ht="31.5">
       <c r="A40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="1">
+        <v>61192</v>
+      </c>
+      <c r="D40" s="8">
+        <v>79983</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I40" s="10">
+        <v>365.625</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0.185</v>
+      </c>
+      <c r="K40" s="11">
+        <f t="shared" si="2"/>
+        <v>67640.625</v>
+      </c>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="1:17" s="12" customFormat="1" ht="31.5">
+      <c r="A41" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C41" s="1">
         <v>60726</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D41" s="8">
         <v>80044</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I40" s="11">
+      <c r="I41" s="10">
         <v>366.66666666700002</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J41" s="1">
         <v>0.28299999999999997</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K41" s="11">
         <f t="shared" si="2"/>
         <v>103766.666666761</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="13" customFormat="1" ht="31.5">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:17" s="12" customFormat="1" ht="31.5">
+      <c r="A42" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C42" s="1">
         <v>60274</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D42" s="8">
         <v>77806</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I41" s="11">
+      <c r="I42" s="10">
         <v>379.16666666700002</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J42" s="1">
         <v>0.217</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K42" s="11">
         <f t="shared" si="2"/>
         <v>82279.166666739009</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="13" customFormat="1" ht="31.5">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:17" s="12" customFormat="1" ht="31.5">
+      <c r="A43" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C43" s="1">
         <v>60400</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D43" s="8">
         <v>78052</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I42" s="11">
+      <c r="I43" s="10">
         <v>266.66666666700002</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J43" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K43" s="11">
         <f t="shared" si="2"/>
         <v>149333.33333352002</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="31.5">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:17" ht="31.5">
+      <c r="A44" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C44" s="1">
         <v>60312</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D44" s="8">
         <v>77950</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I43" s="11">
+      <c r="I44" s="10">
         <v>370</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J44" s="1">
         <v>0.192</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K44" s="11">
         <f t="shared" si="2"/>
         <v>71040</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="31.5">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:17" ht="31.5">
+      <c r="A45" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C45" s="1">
         <v>60520</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D45" s="8">
         <v>78139</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I44" s="11">
+      <c r="I45" s="10">
         <v>375</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J45" s="1">
         <v>0.184</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K45" s="11">
         <f t="shared" si="2"/>
         <v>69000</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="31.5">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:17" ht="31.5">
+      <c r="A46" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C46" s="1">
         <v>60338</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D46" s="8">
         <v>77985</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I45" s="11">
+      <c r="I46" s="10">
         <v>365.625</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J46" s="1">
         <v>0.2</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K46" s="11">
         <f t="shared" si="2"/>
         <v>73125</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="31.5">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:17" ht="31.5">
+      <c r="A47" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C47" s="1">
         <v>60344</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D47" s="8">
         <v>77994</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I46" s="11">
+      <c r="I47" s="10">
         <v>362.5</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J47" s="1">
         <v>0.184</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K47" s="11">
         <f t="shared" si="2"/>
         <v>66700</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="18" customFormat="1" ht="31.5">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:17" s="17" customFormat="1" ht="31.5">
+      <c r="A48" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C48" s="2">
         <v>60377</v>
       </c>
-      <c r="D47" s="16">
+      <c r="D48" s="15">
         <v>78027</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I47" s="10">
+      <c r="I48" s="9">
         <v>385</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J48" s="2">
         <v>0.17799999999999999</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K48" s="3">
         <f t="shared" si="2"/>
         <v>68530</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="31.5">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:11" ht="31.5">
+      <c r="A49" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C49" s="1">
         <v>60287</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D49" s="8">
         <v>77984</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I48" s="11">
+      <c r="I49" s="10">
         <v>365.625</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J49" s="1">
         <v>0.184</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K49" s="11">
         <f t="shared" si="2"/>
         <v>67275</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" ht="31.5">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:11" s="1" customFormat="1" ht="31.5">
+      <c r="A50" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C50" s="1">
         <v>61362</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D50" s="8">
         <v>80259</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I49" s="11">
+      <c r="I50" s="10">
         <v>378.125</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J50" s="1">
         <v>0.185</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K50" s="11">
         <f t="shared" si="2"/>
         <v>69953.125</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" ht="31.5">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:11" s="1" customFormat="1" ht="31.5">
+      <c r="A51" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C51" s="1">
         <v>61272</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D51" s="8">
         <v>80216</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I50" s="11">
+      <c r="I51" s="10">
         <v>371.875</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J51" s="1">
         <v>0.20200000000000001</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K51" s="11">
         <f t="shared" si="2"/>
         <v>75118.75</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="31.5">
-      <c r="A51" s="17" t="s">
+    <row r="52" spans="1:11" ht="31.5">
+      <c r="A52" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C52" s="1">
         <v>62027</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D52" s="8">
         <v>79659</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I51" s="11">
+      <c r="I52" s="10">
         <v>365.625</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J52" s="1">
         <v>0.19900000000000001</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K52" s="11">
         <f t="shared" si="2"/>
         <v>72759.375</v>
       </c>

</xml_diff>